<commit_message>
control dia 27 febrero
</commit_message>
<xml_diff>
--- a/documentacion/Control Tiempo.xlsx
+++ b/documentacion/Control Tiempo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jorge Luis" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>Localizacion en mapas android</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>que me agrege a un vector los prodcutos al darle el boton add</t>
+  </si>
+  <si>
+    <t>crear portafolio</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -602,10 +605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,6 +700,34 @@
       </c>
       <c r="F6">
         <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42062</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>4.5</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42059</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>4.5</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actualizado al 4 de febrero
</commit_message>
<xml_diff>
--- a/documentacion/Control Tiempo.xlsx
+++ b/documentacion/Control Tiempo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Jorge Luis" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
   <si>
     <t>Localizacion en mapas android</t>
   </si>
@@ -118,6 +118,30 @@
   </si>
   <si>
     <t>crear portafolio</t>
+  </si>
+  <si>
+    <t>8 horas</t>
+  </si>
+  <si>
+    <t>organizar lo que ya esta hecho</t>
+  </si>
+  <si>
+    <t>no se nada</t>
+  </si>
+  <si>
+    <t>4 horas</t>
+  </si>
+  <si>
+    <t>NO PUEDO CAPTURAR EL CLICK EN EL HIJO DEL LA LISTA EXPANDIBLE</t>
+  </si>
+  <si>
+    <t>crear clase y formulario usuario</t>
+  </si>
+  <si>
+    <t>Imágenes a utilizar en portafolio</t>
+  </si>
+  <si>
+    <t>crear interfaz de el pedido y carrito</t>
   </si>
 </sst>
 </file>
@@ -159,12 +183,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -450,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,9 +600,64 @@
         <v>28</v>
       </c>
       <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>42065</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42065</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42066</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>0</v>
       </c>
     </row>
@@ -605,10 +686,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,6 +811,36 @@
         <v>100</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>42062</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>42065</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -737,10 +848,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,6 +994,54 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>42065</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="4">
+        <v>6</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>42065</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -890,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,6 +1163,45 @@
         <v>26</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>41700</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>41700</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>41701</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10">
         <v>0</v>
       </c>
     </row>
@@ -1029,14 +1227,14 @@
       <c r="A1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">

</xml_diff>

<commit_message>
interfaz terminada de agregar productos
</commit_message>
<xml_diff>
--- a/documentacion/Control Tiempo.xlsx
+++ b/documentacion/Control Tiempo.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\appDomi\appDomi\documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Jorge Luis" sheetId="1" r:id="rId1"/>
@@ -18,8 +13,11 @@
     <sheet name="Juan carlos" sheetId="4" r:id="rId4"/>
     <sheet name="Deuda" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
   <si>
     <t>Localizacion en mapas android</t>
   </si>
@@ -142,16 +140,38 @@
   </si>
   <si>
     <t>crear interfaz de el pedido y carrito</t>
+  </si>
+  <si>
+    <t>terminar portafolio</t>
+  </si>
+  <si>
+    <t>agregar el pedido a una base de datos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,8 +200,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -195,7 +227,19 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -254,7 +298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -289,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -466,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,22 +520,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="72.7109375" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.85546875" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="9" max="9" width="37.85546875" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="72.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="36.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
+    <col min="9" max="9" width="37.83203125" customWidth="1"/>
+    <col min="10" max="10" width="37.6640625" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -511,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -522,7 +566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>42058</v>
       </c>
@@ -533,7 +577,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -544,7 +588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>42059</v>
       </c>
@@ -561,7 +605,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>42059</v>
       </c>
@@ -575,7 +619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>42062</v>
       </c>
@@ -592,7 +636,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>42062</v>
       </c>
@@ -606,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>42065</v>
       </c>
@@ -624,7 +668,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>42065</v>
       </c>
@@ -644,7 +688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>42066</v>
       </c>
@@ -661,45 +705,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>41704</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>41704</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12">
       <c r="C30" s="2"/>
       <c r="F30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12">
       <c r="A31" s="1"/>
       <c r="C31" s="2"/>
       <c r="F31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12">
       <c r="C32" s="2"/>
       <c r="F32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="39.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.5" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -719,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -730,7 +808,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>42055</v>
       </c>
@@ -741,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -755,7 +833,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -769,7 +847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>42059</v>
       </c>
@@ -783,7 +861,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>42062</v>
       </c>
@@ -797,7 +875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>42059</v>
       </c>
@@ -811,7 +889,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>42062</v>
       </c>
@@ -827,7 +905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="5">
         <v>42065</v>
       </c>
@@ -841,8 +919,39 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>41704</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>41704</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -854,13 +963,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="57.85546875" customWidth="1"/>
+    <col min="2" max="2" width="57.83203125" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -880,7 +989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -891,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>42058</v>
       </c>
@@ -905,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>42058</v>
       </c>
@@ -919,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>42058</v>
       </c>
@@ -933,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>42059</v>
       </c>
@@ -947,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>41697</v>
       </c>
@@ -964,7 +1073,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>41697</v>
       </c>
@@ -978,7 +1087,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="3">
         <v>42062</v>
       </c>
@@ -994,7 +1103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="3">
         <v>42065</v>
       </c>
@@ -1014,7 +1123,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="3">
         <v>42065</v>
       </c>
@@ -1034,7 +1143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1044,6 +1153,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1055,15 +1169,15 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="52.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="52.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1083,7 +1197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>42055</v>
       </c>
@@ -1097,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>42058</v>
       </c>
@@ -1105,7 +1219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="3">
         <v>42058</v>
       </c>
@@ -1121,7 +1235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>42059</v>
       </c>
@@ -1135,7 +1249,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>41697</v>
       </c>
@@ -1149,7 +1263,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>41697</v>
       </c>
@@ -1166,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>41700</v>
       </c>
@@ -1180,7 +1294,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>41700</v>
       </c>
@@ -1191,7 +1305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>41701</v>
       </c>
@@ -1207,6 +1321,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1218,12 +1337,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -1236,7 +1355,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>41694</v>
       </c>
@@ -1247,7 +1366,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>41697</v>
       </c>
@@ -1264,5 +1383,10 @@
     <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
app movil sin barra buscar
</commit_message>
<xml_diff>
--- a/documentacion/Control Tiempo.xlsx
+++ b/documentacion/Control Tiempo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20500" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Jorge Luis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>Localizacion en mapas android</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>agregar el pedido a una base de datos</t>
+  </si>
+  <si>
+    <t>ninguno</t>
+  </si>
+  <si>
+    <t>indicar en el boton el total en pedidos</t>
+  </si>
+  <si>
+    <t>crear interfaces y clases para carrito</t>
   </si>
 </sst>
 </file>
@@ -200,8 +209,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -227,19 +254,37 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="31">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -520,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -733,6 +778,62 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5">
+        <v>42072</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5">
+        <v>42072</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5">
+        <v>42072</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="5">
+        <v>42072</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+    </row>
     <row r="29" spans="1:12">
       <c r="A29" s="1"/>
     </row>
@@ -764,10 +865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -942,6 +1043,23 @@
       </c>
       <c r="C12">
         <v>5</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>41708</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -960,7 +1078,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1144,15 +1262,28 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="A12" s="5">
+        <v>42072</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="6">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1331,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1374,6 +1505,17 @@
         <v>23</v>
       </c>
       <c r="E3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>41707</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
         <v>6000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
direcciones add y update
</commit_message>
<xml_diff>
--- a/documentacion/Control Tiempo.xlsx
+++ b/documentacion/Control Tiempo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14360" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Jorge Luis" sheetId="1" r:id="rId1"/>
@@ -652,7 +652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1614,7 +1614,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1733,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1902,6 +1902,91 @@
       </c>
       <c r="E8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1">
+        <v>42088</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1">
+        <v>42089</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1">
+        <v>42090</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1">
+        <v>42100</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1">
+        <v>42100</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>